<commit_message>
Update sta_class with USGS Vs30 as reference
</commit_message>
<xml_diff>
--- a/result/sta_class.xlsx
+++ b/result/sta_class.xlsx
@@ -15,14 +15,14 @@
     <sheet name="sta" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sta!$A$1:$L$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sta!$A$1:$M$68</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
   <si>
     <t>BCVB</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Average Vs30</t>
+  </si>
+  <si>
+    <t>Reference Vs30 (USGS)</t>
   </si>
 </sst>
 </file>
@@ -836,16 +839,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>142079</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>104121</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>227804</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142221</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -862,7 +865,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7181850" y="1162050"/>
+          <a:off x="10925175" y="1390650"/>
           <a:ext cx="6371429" cy="5228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1179,7 +1182,7 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,6 +1225,9 @@
         <v>88</v>
       </c>
       <c r="L1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1262,6 +1268,9 @@
         <f>IF(I2="CL-I","&gt;600 m/s",IF(I2="300-600 m/s","C+D",IF(I2="CL-III","200-300 m/s",IF(I2="CL-IV","&lt; 200 m/s",IF(I2="CL-V","&gt; 600 m/s","???")))))</f>
         <v>&gt;600 m/s</v>
       </c>
+      <c r="L2">
+        <v>851</v>
+      </c>
       <c r="P2" t="s">
         <v>78</v>
       </c>
@@ -1303,6 +1312,9 @@
         <f t="shared" ref="K3:K10" si="2">IF(I3="CL-I","&gt;600 m/s",IF(I3="300-600 m/s","C+D",IF(I3="CL-III","200-300 m/s",IF(I3="CL-IV","&lt; 200 m/s",IF(I3="CL-V","&gt; 600 m/s","???")))))</f>
         <v>&gt;600 m/s</v>
       </c>
+      <c r="L3">
+        <v>223</v>
+      </c>
       <c r="P3" t="s">
         <v>79</v>
       </c>
@@ -1344,6 +1356,9 @@
         <f t="shared" si="2"/>
         <v>&gt;600 m/s</v>
       </c>
+      <c r="L4">
+        <v>713</v>
+      </c>
       <c r="P4" t="s">
         <v>80</v>
       </c>
@@ -1385,6 +1400,9 @@
         <f t="shared" si="2"/>
         <v>&lt; 200 m/s</v>
       </c>
+      <c r="L5">
+        <v>900</v>
+      </c>
       <c r="P5" t="s">
         <v>81</v>
       </c>
@@ -1426,6 +1444,9 @@
         <f t="shared" si="2"/>
         <v>200-300 m/s</v>
       </c>
+      <c r="L6">
+        <v>757</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1464,6 +1485,9 @@
         <f t="shared" si="2"/>
         <v>???</v>
       </c>
+      <c r="L7">
+        <v>306</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1502,6 +1526,9 @@
         <f t="shared" si="2"/>
         <v>&gt;600 m/s</v>
       </c>
+      <c r="L8">
+        <v>339</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1540,6 +1567,9 @@
         <f t="shared" si="2"/>
         <v>&gt;600 m/s</v>
       </c>
+      <c r="L9">
+        <v>539</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1577,7 +1607,10 @@
         <f t="shared" si="2"/>
         <v>???</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <v>759</v>
+      </c>
+      <c r="M10" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1609,7 +1642,7 @@
       <c r="J11" t="s">
         <v>76</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1649,7 +1682,10 @@
         <f t="shared" ref="K12:K28" si="3">IF(I12="CL-I","&gt;600 m/s",IF(I12="300-600 m/s","C+D",IF(I12="CL-III","200-300 m/s",IF(I12="CL-IV","&lt; 200 m/s",IF(I12="CL-V","&gt; 600 m/s","???")))))</f>
         <v>???</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12">
+        <v>606</v>
+      </c>
+      <c r="M12" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1690,6 +1726,9 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
+      <c r="L13">
+        <v>392</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1728,6 +1767,9 @@
         <f t="shared" si="3"/>
         <v>&lt; 200 m/s</v>
       </c>
+      <c r="L14">
+        <v>615</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1765,7 +1807,10 @@
         <f t="shared" si="3"/>
         <v>&gt; 600 m/s</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15">
+        <v>783</v>
+      </c>
+      <c r="M15" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1806,8 +1851,11 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1843,11 +1891,14 @@
         <f t="shared" si="3"/>
         <v>???</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17">
+        <v>475</v>
+      </c>
+      <c r="M17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1884,8 +1935,11 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1922,8 +1976,11 @@
         <f t="shared" si="3"/>
         <v>&lt; 200 m/s</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1960,8 +2017,11 @@
         <f t="shared" si="3"/>
         <v>&lt; 200 m/s</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1998,8 +2058,11 @@
         <f t="shared" si="3"/>
         <v>&lt; 200 m/s</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2036,8 +2099,11 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2074,8 +2140,11 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2112,8 +2181,11 @@
         <f t="shared" si="3"/>
         <v>&lt; 200 m/s</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2150,8 +2222,11 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2187,11 +2262,14 @@
         <f t="shared" si="3"/>
         <v>&gt; 600 m/s</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26">
+        <v>644</v>
+      </c>
+      <c r="M26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2228,8 +2306,11 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2266,8 +2347,11 @@
         <f t="shared" si="3"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2298,11 +2382,11 @@
       <c r="J29" t="s">
         <v>76</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2339,8 +2423,11 @@
         <f t="shared" ref="K30:K33" si="4">IF(I30="CL-I","&gt;600 m/s",IF(I30="300-600 m/s","C+D",IF(I30="CL-III","200-300 m/s",IF(I30="CL-IV","&lt; 200 m/s",IF(I30="CL-V","&gt; 600 m/s","???")))))</f>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2377,8 +2464,11 @@
         <f t="shared" si="4"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2415,8 +2505,11 @@
         <f t="shared" si="4"/>
         <v>???</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2453,8 +2546,11 @@
         <f t="shared" si="4"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2485,11 +2581,14 @@
       <c r="J34" t="s">
         <v>76</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34">
+        <v>700</v>
+      </c>
+      <c r="M34" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2526,8 +2625,11 @@
         <f t="shared" ref="K35:K40" si="5">IF(I35="CL-I","&gt;600 m/s",IF(I35="300-600 m/s","C+D",IF(I35="CL-III","200-300 m/s",IF(I35="CL-IV","&lt; 200 m/s",IF(I35="CL-V","&gt; 600 m/s","???")))))</f>
         <v>???</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2564,8 +2666,11 @@
         <f t="shared" si="5"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2601,11 +2706,14 @@
         <f t="shared" si="5"/>
         <v>&gt; 600 m/s</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37">
+        <v>617</v>
+      </c>
+      <c r="M37" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2641,11 +2749,14 @@
         <f t="shared" si="5"/>
         <v>???</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38">
+        <v>392</v>
+      </c>
+      <c r="M38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2682,8 +2793,11 @@
         <f t="shared" si="5"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2719,11 +2833,14 @@
         <f t="shared" si="5"/>
         <v>???</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L40">
+        <v>556</v>
+      </c>
+      <c r="M40" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2754,11 +2871,14 @@
       <c r="J41" t="s">
         <v>76</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L41">
+        <v>489</v>
+      </c>
+      <c r="M41" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2795,8 +2915,11 @@
         <f t="shared" ref="K42:K68" si="6">IF(I42="CL-I","&gt;600 m/s",IF(I42="300-600 m/s","C+D",IF(I42="CL-III","200-300 m/s",IF(I42="CL-IV","&lt; 200 m/s",IF(I42="CL-V","&gt; 600 m/s","???")))))</f>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2833,8 +2956,11 @@
         <f t="shared" si="6"/>
         <v>&lt; 200 m/s</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2871,8 +2997,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2909,8 +3038,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2947,8 +3079,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2985,8 +3120,11 @@
         <f t="shared" si="6"/>
         <v>&lt; 200 m/s</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3023,8 +3161,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3061,8 +3202,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3099,8 +3243,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3137,8 +3284,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3175,8 +3325,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3213,8 +3366,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3251,8 +3407,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3289,8 +3448,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3327,8 +3489,11 @@
         <f t="shared" si="6"/>
         <v>???</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3365,8 +3530,11 @@
         <f t="shared" si="6"/>
         <v>???</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3403,8 +3571,11 @@
         <f t="shared" si="6"/>
         <v>???</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3441,8 +3612,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3479,8 +3653,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3516,11 +3693,14 @@
         <f t="shared" si="6"/>
         <v>&gt; 600 m/s</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L61">
+        <v>720</v>
+      </c>
+      <c r="M61" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3556,11 +3736,14 @@
         <f t="shared" si="6"/>
         <v>&gt; 600 m/s</v>
       </c>
-      <c r="L62" t="s">
+      <c r="L62">
+        <v>698</v>
+      </c>
+      <c r="M62" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3596,11 +3779,14 @@
         <f t="shared" si="6"/>
         <v>&gt; 600 m/s</v>
       </c>
-      <c r="L63" t="s">
+      <c r="L63">
+        <v>570</v>
+      </c>
+      <c r="M63" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3637,8 +3823,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3675,8 +3864,11 @@
         <f t="shared" si="6"/>
         <v>&gt;600 m/s</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3713,8 +3905,11 @@
         <f t="shared" si="6"/>
         <v>???</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3751,8 +3946,11 @@
         <f t="shared" si="6"/>
         <v>&lt; 200 m/s</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3789,13 +3987,11 @@
         <f t="shared" si="6"/>
         <v>&lt; 200 m/s</v>
       </c>
+      <c r="L68">
+        <v>759</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L68">
-    <sortState ref="A2:K68">
-      <sortCondition ref="A1:A68"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>